<commit_message>
Unittests fuer Methoden 'insert_arbeitslosenversicherungsbeitraege' und 'insert_rentenversicherungsbeitraege' geschrieben
</commit_message>
<xml_diff>
--- a/src/test/testdaten_insert_arbeitslosenversicherungsbeitraege/Arbeitslosenversicherungsbeitraege - andere Beitragssaetze.xlsx
+++ b/src/test/testdaten_insert_arbeitslosenversicherungsbeitraege/Arbeitslosenversicherungsbeitraege - andere Beitragssaetze.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_arbeitslosenversicherungsbeitraege\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A79E5089-C1A0-4438-B250-D8DBCBCFC013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D363DA-8E56-404E-89BB-8B7D49003FCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4992" yWindow="1728" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <t>Eintragungsdatum</t>
   </si>
   <si>
-    <t>15.12.2023</t>
+    <t>17.12.2023</t>
   </si>
 </sst>
 </file>
@@ -380,7 +380,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>